<commit_message>
unit test? question added
</commit_message>
<xml_diff>
--- a/TimeSheet-Imran.xlsx
+++ b/TimeSheet-Imran.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Task Name</t>
   </si>
@@ -60,12 +60,15 @@
   <si>
     <t>Tank Dispatch</t>
   </si>
+  <si>
+    <t>Unit Tested?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,13 +137,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -202,7 +205,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -234,10 +237,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -269,7 +271,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -445,14 +446,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="40.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="40.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="82" bestFit="1" customWidth="1"/>
@@ -463,21 +464,22 @@
     <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="139.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" ht="40.5" customHeight="1">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="40.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,9 +507,12 @@
       <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:10" ht="40.5" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B3">
@@ -526,8 +531,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:10" ht="40.5" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B4">
@@ -556,24 +561,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>